<commit_message>
did first event analysis
</commit_message>
<xml_diff>
--- a/data overview.xlsx
+++ b/data overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasborn/Desktop/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasborn/Desktop/analysis/ASCAM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4A0949-F6A7-AB44-894A-969ECE09893D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BA58F0-AD10-074B-9578-3EA2C1009968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="38400" windowHeight="19840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="38400" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T1 in EDTA + CTZ" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="168">
   <si>
     <t>File name</t>
   </si>
@@ -481,10 +481,70 @@
     <t>0.  , -0.53, -1.1 , -1.63, -2.17</t>
   </si>
   <si>
-    <t>0.  , -0.58, -1.19, -1.77, -2.36</t>
-  </si>
-  <si>
     <t>0. ,-0.59, -1.22, -1.82, -2.42</t>
+  </si>
+  <si>
+    <t>0-46</t>
+  </si>
+  <si>
+    <t>all?</t>
+  </si>
+  <si>
+    <t>344-466</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>1-243,![114,115,156,164-166,191,201,204,237]</t>
+  </si>
+  <si>
+    <t>skipped episode 166 because</t>
+  </si>
+  <si>
+    <t>skipped episode 329 because</t>
+  </si>
+  <si>
+    <t>skipped episode 331 because</t>
+  </si>
+  <si>
+    <t>skipped episode 345 because</t>
+  </si>
+  <si>
+    <t>skipped episode 347 because</t>
+  </si>
+  <si>
+    <t>skipped episode 356 because</t>
+  </si>
+  <si>
+    <t>skipped episode 364 because</t>
+  </si>
+  <si>
+    <t>skipped episode 370 because</t>
+  </si>
+  <si>
+    <t>skipped episode 379 because</t>
+  </si>
+  <si>
+    <t>skipped episode 400 because</t>
+  </si>
+  <si>
+    <t>skipped episode 406 because</t>
+  </si>
+  <si>
+    <t>skipped episode 791 because no events detected</t>
+  </si>
+  <si>
+    <t>skipped episode 1224 because no events detected</t>
+  </si>
+  <si>
+    <t>skipped episode 1229 because no events detected</t>
+  </si>
+  <si>
+    <t>skipped episode 1231 because no events detected</t>
+  </si>
+  <si>
+    <t>skipped episode 1356 because no events detected</t>
   </si>
 </sst>
 </file>
@@ -880,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="134" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="134" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -974,6 +1034,9 @@
       <c r="M2" t="s">
         <v>143</v>
       </c>
+      <c r="N2" t="s">
+        <v>147</v>
+      </c>
       <c r="O2" t="s">
         <v>22</v>
       </c>
@@ -1018,6 +1081,9 @@
       <c r="M3" t="s">
         <v>144</v>
       </c>
+      <c r="N3" s="5" t="s">
+        <v>148</v>
+      </c>
       <c r="O3" t="s">
         <v>23</v>
       </c>
@@ -1061,6 +1127,9 @@
       </c>
       <c r="M4" t="s">
         <v>145</v>
+      </c>
+      <c r="N4" t="s">
+        <v>149</v>
       </c>
       <c r="O4" t="s">
         <v>27</v>
@@ -1190,10 +1259,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BL12"/>
+  <dimension ref="A1:BL19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="129" zoomScalePageLayoutView="129" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView zoomScale="129" zoomScaleNormal="129" zoomScalePageLayoutView="129" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1380,7 +1449,9 @@
       <c r="M4" t="s">
         <v>143</v>
       </c>
-      <c r="N4"/>
+      <c r="N4" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="O4" t="s">
         <v>27</v>
       </c>
@@ -1744,10 +1815,14 @@
         <v>33</v>
       </c>
       <c r="M9" t="s">
-        <v>146</v>
-      </c>
-      <c r="N9"/>
-      <c r="O9"/>
+        <v>143</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="O9" t="s">
+        <v>152</v>
+      </c>
       <c r="P9"/>
       <c r="Q9"/>
       <c r="R9"/>
@@ -1832,6 +1907,9 @@
       <c r="L10" t="s">
         <v>45</v>
       </c>
+      <c r="O10" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="11" spans="1:64" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
@@ -1869,7 +1947,9 @@
       </c>
       <c r="M11"/>
       <c r="N11"/>
-      <c r="O11"/>
+      <c r="O11" t="s">
+        <v>154</v>
+      </c>
       <c r="P11"/>
       <c r="Q11"/>
       <c r="R11"/>
@@ -1955,7 +2035,60 @@
         <v>71</v>
       </c>
       <c r="M12" t="s">
-        <v>147</v>
+        <v>146</v>
+      </c>
+      <c r="O12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="O13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="M14" t="s">
+        <v>163</v>
+      </c>
+      <c r="O14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="M15" t="s">
+        <v>164</v>
+      </c>
+      <c r="O15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="M16" t="s">
+        <v>165</v>
+      </c>
+      <c r="O16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="M17" t="s">
+        <v>166</v>
+      </c>
+      <c r="O17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="M18" t="s">
+        <v>167</v>
+      </c>
+      <c r="O18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="O19" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>